<commit_message>
Fix & Update: Adjusted "NCSC CAF notes.md" & filled in half of the matrix in "gap-analysis-template.xlsx"
</commit_message>
<xml_diff>
--- a/templates/gap-analysis-template.xlsx
+++ b/templates/gap-analysis-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\ALL MY FILES\Documents\Personal Coding\Cybersecurity projects\controls-gap-analysis\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF6DE55-EE45-4114-BE09-53188C1CC4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78E3662-A392-4E27-B6EA-E812C5D6AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Control Area</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Current Control (H&amp;F)</t>
   </si>
   <si>
-    <t>Framework Requirement (CAF / ISO 27001)</t>
-  </si>
-  <si>
     <t>Gap</t>
   </si>
   <si>
@@ -53,13 +50,218 @@
   </si>
   <si>
     <t>Recommendation</t>
+  </si>
+  <si>
+    <t>Framework Requirement (CAF / ISO 27001 / Data Protection Act 2018)</t>
+  </si>
+  <si>
+    <t>Data Protection</t>
+  </si>
+  <si>
+    <t>H&amp;F council trains its staff so "they're aware how to safely handle information".</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective B6 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Staff Awareness and Training</t>
+    </r>
+  </si>
+  <si>
+    <t>No evidence or mention of the type of training to handle data safely</t>
+  </si>
+  <si>
+    <t>Medium - Human error can occur, and impact on system can vary</t>
+  </si>
+  <si>
+    <t>System Management</t>
+  </si>
+  <si>
+    <t>H&amp;F council regularly tests their IT system and procedures, to reduce vulnerabilities.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective B4 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>System Security</t>
+    </r>
+  </si>
+  <si>
+    <t>No Gaps</t>
+  </si>
+  <si>
+    <t>H&amp;F should mention the type/form/name of training they perform on their website, which verifies a clear process in staff training.</t>
+  </si>
+  <si>
+    <t>It is best to keep private the IT systems because they are used to store very personal and sensitive information of a significant population within a community.</t>
+  </si>
+  <si>
+    <t>Low - Regularly testing IT systems help confirm procedures and frameworks are being implemented, and ensures weaknesses of system are bing checked.</t>
+  </si>
+  <si>
+    <t>Access Control</t>
+  </si>
+  <si>
+    <t>To log into your personal portal, you have enter your email and password of your account.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective B2 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Identity And Access Control</t>
+    </r>
+  </si>
+  <si>
+    <t>Only one level of verification to access account, which is the password entered.</t>
+  </si>
+  <si>
+    <t>H&amp;F should add an extra step of authentication/verification at least that could prevent unauthorised user to having access from a login, such as "Enter code received in email", or entering a "Secret Answer".</t>
+  </si>
+  <si>
+    <t>User Control</t>
+  </si>
+  <si>
+    <t>40 minutes might be a bit too long for no activity timing.</t>
+  </si>
+  <si>
+    <t>Low - An unauthorised user can go onto the device with the active form and tamper with the details put on the form.</t>
+  </si>
+  <si>
+    <t>H&amp;F should make it shorter to 25 or 30 minutes to reduce the chance of an active activity being spotted by an unauthorised user. It also alerts the actual user to be aware to come back as soon as possible if they have not been active for some time.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective B3 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Security</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>When entering the "Am I registered to vote in Hammersmith &amp; Fulham?" from in the portal, I am greeted with a red message saying:   "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>For security reasons, if there is no activity on this site for 40 minutes you will be logged out, and your form will not be saved.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>".</t>
+    </r>
+  </si>
+  <si>
+    <t>Data Management</t>
+  </si>
+  <si>
+    <t>On the "Digital services privacy notice" page of the council's website, the council lists out the personal information of residents they collect and process.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective A1 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Governance</t>
+    </r>
+  </si>
+  <si>
+    <t>Low - Council is communicating with residents about what personal information is processed by themselves.</t>
+  </si>
+  <si>
+    <t>H&amp;F should continue to keep this practice as its residents know about their personal information being processed, which is a practice in relation to the Data Protection Act 2018.</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>On the "Cookies and IP addresses" page of the council, they explain the Google Analytics cookies used are to collect information on how their sites are used, to compile reports and help improve the sites.</t>
+  </si>
+  <si>
+    <t>Low - Council explaining the purpose as to why they have cookies keeping track of how user interacts with the site.</t>
+  </si>
+  <si>
+    <t>H&amp;F should continue to this good practice.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective A3 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Asset Management</t>
+    </r>
+  </si>
+  <si>
+    <t>High - If account is breached, unauthroised user can access personal information of account, such as phone number &amp; address. Can result in massive consequences.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +297,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -123,11 +340,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -465,301 +689,373 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C1E297-21ED-43A1-9A9E-ACD768065ED2}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="39" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update: Finished and finalised the table matrix
</commit_message>
<xml_diff>
--- a/templates/gap-analysis-template.xlsx
+++ b/templates/gap-analysis-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\ALL MY FILES\Documents\Personal Coding\Cybersecurity projects\controls-gap-analysis\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E692057B-DBBB-4538-B0D6-A09613826068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B800CEC-04B6-42A9-ACB6-F4D68F8F13A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
+    <workbookView xWindow="14295" yWindow="105" windowWidth="14610" windowHeight="15480" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Control Area</t>
   </si>
@@ -77,15 +77,9 @@
     </r>
   </si>
   <si>
-    <t>No evidence or mention of the type of training to handle data safely</t>
-  </si>
-  <si>
     <t>Medium - Human error can occur, and impact on system can vary</t>
   </si>
   <si>
-    <t>System Management</t>
-  </si>
-  <si>
     <t>H&amp;F council regularly tests their IT system and procedures, to reduce vulnerabilities.</t>
   </si>
   <si>
@@ -108,21 +102,9 @@
     <t>No Gaps</t>
   </si>
   <si>
-    <t>H&amp;F should mention the type/form/name of training they perform on their website, which verifies a clear process in staff training.</t>
-  </si>
-  <si>
-    <t>It is best to keep private the IT systems because they are used to store very personal and sensitive information of a significant population within a community.</t>
-  </si>
-  <si>
-    <t>Low - Regularly testing IT systems help confirm procedures and frameworks are being implemented, and ensures weaknesses of system are bing checked.</t>
-  </si>
-  <si>
     <t>Access Control</t>
   </si>
   <si>
-    <t>To log into your personal portal, you have enter your email and password of your account.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective B2 - </t>
     </r>
@@ -139,22 +121,7 @@
     </r>
   </si>
   <si>
-    <t>Only one level of verification to access account, which is the password entered.</t>
-  </si>
-  <si>
     <t>H&amp;F should add an extra step of authentication/verification at least that could prevent unauthorised user to having access from a login, such as "Enter code received in email", or entering a "Secret Answer".</t>
-  </si>
-  <si>
-    <t>User Control</t>
-  </si>
-  <si>
-    <t>40 minutes might be a bit too long for no activity timing.</t>
-  </si>
-  <si>
-    <t>Low - An unauthorised user can go onto the device with the active form and tamper with the details put on the form.</t>
-  </si>
-  <si>
-    <t>H&amp;F should make it shorter to 25 or 30 minutes to reduce the chance of an active activity being spotted by an unauthorised user. It also alerts the actual user to be aware to come back as soon as possible if they have not been active for some time.</t>
   </si>
   <si>
     <r>
@@ -220,24 +187,9 @@
     </r>
   </si>
   <si>
-    <t>Low - Council is communicating with residents about what personal information is processed by themselves.</t>
-  </si>
-  <si>
-    <t>H&amp;F should continue to keep this practice as its residents know about their personal information being processed, which is a practice in relation to the Data Protection Act 2018.</t>
-  </si>
-  <si>
-    <t>Cookies</t>
-  </si>
-  <si>
     <t>On the "Cookies and IP addresses" page of the council, they explain the Google Analytics cookies used are to collect information on how their sites are used, to compile reports and help improve the sites.</t>
   </si>
   <si>
-    <t>Low - Council explaining the purpose as to why they have cookies keeping track of how user interacts with the site.</t>
-  </si>
-  <si>
-    <t>H&amp;F should continue to this good practice.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective A3 - </t>
     </r>
@@ -254,7 +206,229 @@
     </r>
   </si>
   <si>
-    <t>High - If account is breached, unauthroised user can access personal information of account, such as phone number &amp; address. Can result in massive consequences.</t>
+    <r>
+      <t xml:space="preserve">Resident Experience Team manages </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FOI, EIR, SAR, IRR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ensuring compliance with legal requirements. The Information Management Team ensures compliance with</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> FOIA 2000, EIR 2004,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Data Protection Act 1998.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ISO 27001 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clause 4 Context of Organisation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Scope</t>
+    </r>
+  </si>
+  <si>
+    <t>When you log in to your personal portal, you can search for rateable values associated with a postcode or an address.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ISO 27001 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clause 7 Support</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Documented Information</t>
+    </r>
+  </si>
+  <si>
+    <t>H&amp;F's control room consists of around 1850 cameras throughout the borough, and have radio communications with the police. CCTV is used to ensure reducing crime rates. Residents can access CCTV footage according to their rights, and have to fill a form consisting of personal information and signing the application form.</t>
+  </si>
+  <si>
+    <r>
+      <t>ISO 27001 Annex A Control -</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Physical Controls</t>
+    </r>
+  </si>
+  <si>
+    <t>ISO 27001 Annex A Control - Physical Controls</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Access Procedures</t>
+  </si>
+  <si>
+    <t>Low - H&amp;F Council checked their records about me and verified that I have entered the correct address. You also need to log in to your account to do this, which serves as a barrier and verifier before checking your registration.</t>
+  </si>
+  <si>
+    <t>Residual Risk</t>
+  </si>
+  <si>
+    <t>Medium - H&amp;F does mention reasons as to why they have the CCTV being watched 24/7. You access parts of it if you verify your details, which are compared to the records they have. However, privacy concerns arise due to non-stop activity monitoring, which can be perceived as intrusive.</t>
+  </si>
+  <si>
+    <t>Pending council response</t>
+  </si>
+  <si>
+    <t>No evidence of training type</t>
+  </si>
+  <si>
+    <t>Single-factor login, which is the password</t>
+  </si>
+  <si>
+    <t>40 minutes timeout could be too long to prevent misuse.</t>
+  </si>
+  <si>
+    <t>Viewing rateable value  of other property to public</t>
+  </si>
+  <si>
+    <t>H&amp;F still have to comply with the law and therefore should continue to disclose the rateable values of their properties to the public.</t>
+  </si>
+  <si>
+    <t>When checking to see if registered to vote, the form asks you to fill your name, telephone number, email, postcode/address and the date moved to it. You then verify you are that person and not having unauthorised access by ticking the box. I filled this up and received an email confirming I am registered at the address I filled.</t>
+  </si>
+  <si>
+    <t>Low - Regularly testing IT systems help confirm procedures and frameworks are being implemented, and ensures weaknesses of system are being checked.</t>
+  </si>
+  <si>
+    <t>ISO 27001 - Clause 5 Leadership - Roles, Responsibilities &amp; Authorities</t>
+  </si>
+  <si>
+    <t>Privacy concerns from 24/7 monitoring, and no backup system</t>
+  </si>
+  <si>
+    <t>H&amp;F should add the type/form/name of training they perform on their website, which verifies a clear process in staff training.</t>
+  </si>
+  <si>
+    <t>H&amp;F should implement a shorter timeout (25 or 30 minutes) to reduce the chance of an active activity being spotted by an unauthorised user. It also alerts the actual user to be aware that they should return as soon as possible if they have been inactive at some point.</t>
+  </si>
+  <si>
+    <t>H&amp;F must continue to maintain this practice, as its residents are aware of their personal information being processed, which is a requirement under the Data Protection Act 2018.</t>
+  </si>
+  <si>
+    <t>H&amp;F must ensure that the records about their residents are up to date at all times, as required by the Data Protection Act 2018. Credit to them, they do attempt this by holding an annual canvass, contacting every property in the borough and checking for changes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H&amp;F council must continue to maintain regular testing of its systems to mitigate potential cybersecurity risks. However, details of the security workers shouldn't be disclosed for security reasons, as they manage personal and sensitive data.</t>
+  </si>
+  <si>
+    <t>H&amp;F must continue this good practice.</t>
+  </si>
+  <si>
+    <t>To log into your personal portal, you have to enter your email and password of your account.</t>
+  </si>
+  <si>
+    <t>Low - An unauthorised user can access the device with the active form and tamper with the details entered on the form.</t>
+  </si>
+  <si>
+    <t>Low - Council is communicating with residents about what they process personal information.</t>
+  </si>
+  <si>
+    <t>Low - Council explaining the purpose of why they have cookies, keeping track of how user interacts with the site.</t>
+  </si>
+  <si>
+    <t>Medium - Council has a dedicated team that ensures data protection complies with legal procedures. There is still a risk of an insider who could abuse or exceed their existing power.</t>
+  </si>
+  <si>
+    <t>Low - In the UK, a rateable value must be shown for business properties, demonstrating that H&amp;F can distinguish between personal and mandated public data. However, anyone in the portal can access a rateable value as long as they enter an address.</t>
+  </si>
+  <si>
+    <t>The H&amp;F council mentions reasons for having non-stop CCTV, but that's a 24/7  intrusion which compromises privacy. If not done, H&amp;F must implement a backup system for their CCTV in the event of a shutdown.</t>
+  </si>
+  <si>
+    <t>H&amp;F must continue to comply with laws regularly to ensure they meet the necessary data security procedures. Breaching the law can have serious consequences such as fines &amp; distrust from the public.</t>
+  </si>
+  <si>
+    <t>High - High – Single-factor login could result in a user’s personal data being breached and gathered. Can result in massive consequences.</t>
   </si>
 </sst>
 </file>
@@ -313,7 +487,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +498,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -340,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -352,6 +532,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -692,7 +875,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,8 +883,8 @@
     <col min="1" max="1" width="25.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="54.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="50.7109375" style="4" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -740,162 +923,234 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="F11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>

</xml_diff>

<commit_message>
Started new "Findings" section in Report Word doc, & made adjustments to matrix.
</commit_message>
<xml_diff>
--- a/templates/gap-analysis-template.xlsx
+++ b/templates/gap-analysis-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\ALL MY FILES\Documents\Personal Coding\Cybersecurity projects\controls-gap-analysis\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E55A5C9-5968-41F5-988B-80BB9B6A7B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD8AD9A-4A4D-4B70-8714-BA12129BDBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="105" windowWidth="14610" windowHeight="15480" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,12 +341,6 @@
     <t>ISO 27001 Annex A Control - Physical Controls</t>
   </si>
   <si>
-    <t>Data Analysis</t>
-  </si>
-  <si>
-    <t>Access Procedures</t>
-  </si>
-  <si>
     <t>Low - H&amp;F Council checked their records about me and verified that I have entered the correct address. You also need to log in to your account to do this, which serves as a barrier and verifier before checking your registration.</t>
   </si>
   <si>
@@ -398,18 +392,6 @@
     <t>H&amp;F must ensure that the records about their residents are up to date at all times, as required by the Data Protection Act 2018. Credit to them, they do attempt this by holding an annual canvass, contacting every property in the borough and checking for changes.</t>
   </si>
   <si>
-    <t xml:space="preserve"> H&amp;F council must continue to maintain regular testing of its systems to mitigate potential cybersecurity risks. However, details of the security workers shouldn't be disclosed for security reasons, as they manage personal and sensitive data.</t>
-  </si>
-  <si>
-    <t>H&amp;F must continue this good practice.</t>
-  </si>
-  <si>
-    <t>To log into your personal portal, you have to enter your email and password of your account.</t>
-  </si>
-  <si>
-    <t>Low - An unauthorised user can access the device with the active form and tamper with the details entered on the form.</t>
-  </si>
-  <si>
     <t>Low - Council is communicating with residents about what they process personal information.</t>
   </si>
   <si>
@@ -428,7 +410,25 @@
     <t>H&amp;F must continue to comply with laws regularly to ensure they meet the necessary data security procedures. Breaching the law can have serious consequences such as fines &amp; distrust from the public.</t>
   </si>
   <si>
-    <t>High - High – Single-factor login could result in a user’s personal data being breached and gathered. Can result in massive consequences.</t>
+    <t>Surveilance</t>
+  </si>
+  <si>
+    <t>Organisational Procedures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H&amp;F council must continue to maintain regular testing of its systems to mitigate potential cybersecurity risks. However, any details about the security workers shouldn't be disclosed for security reasons (structure, personnel), as they manage personal and sensitive data.</t>
+  </si>
+  <si>
+    <t>To log into your personal portal, you have to enter your correct email and password of your account.</t>
+  </si>
+  <si>
+    <t>High – Single-factor login could result in a user’s personal data being breached and gathered. Can result in massive consequences.</t>
+  </si>
+  <si>
+    <t>Medium - An unauthorised user can access the device with the active form and tamper with the details entered on the form.</t>
+  </si>
+  <si>
+    <t>H&amp;F must continue this good practice at all times.</t>
   </si>
 </sst>
 </file>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C1E297-21ED-43A1-9A9E-ACD768065ED2}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,13 +923,13 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -946,10 +946,10 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -957,16 +957,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -983,13 +983,13 @@
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1006,15 +1006,15 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
@@ -1026,10 +1026,10 @@
         <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1040,16 +1040,16 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,13 +1063,13 @@
         <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>26</v>
@@ -1086,15 +1086,15 @@
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
@@ -1103,53 +1103,53 @@
         <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update: Made changes to the matrix, and starting wrting paragraphs about findings from matrix
</commit_message>
<xml_diff>
--- a/templates/gap-analysis-template.xlsx
+++ b/templates/gap-analysis-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\ALL MY FILES\Documents\Personal Coding\Cybersecurity projects\controls-gap-analysis\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD8AD9A-4A4D-4B70-8714-BA12129BDBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E549918-940C-4CC6-A618-98AB4544759A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
+    <workbookView xWindow="14340" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,9 +401,6 @@
     <t>Medium - Council has a dedicated team that ensures data protection complies with legal procedures. There is still a risk of an insider who could abuse or exceed their existing power.</t>
   </si>
   <si>
-    <t>Low - In the UK, a rateable value must be shown for business properties, demonstrating that H&amp;F can distinguish between personal and mandated public data. However, anyone in the portal can access a rateable value as long as they enter an address.</t>
-  </si>
-  <si>
     <t>The H&amp;F council mentions reasons for having non-stop CCTV, but that's a 24/7  intrusion which compromises privacy. If not done, H&amp;F must implement a backup system for their CCTV in the event of a shutdown.</t>
   </si>
   <si>
@@ -429,6 +426,9 @@
   </si>
   <si>
     <t>H&amp;F must continue this good practice at all times.</t>
+  </si>
+  <si>
+    <t>Low - Rateable values of property by law can be viewed by the public.</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,12 +498,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -534,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -874,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C1E297-21ED-43A1-9A9E-ACD768065ED2}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,7 +943,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -957,7 +951,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -966,7 +960,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -986,7 +980,7 @@
         <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>44</v>
@@ -1029,7 +1023,7 @@
         <v>48</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1049,7 +1043,7 @@
         <v>49</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1066,7 +1060,7 @@
         <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>38</v>
@@ -1094,7 +1088,7 @@
     </row>
     <row r="11" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
@@ -1109,12 +1103,12 @@
         <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>33</v>
@@ -1134,7 +1128,7 @@
     </row>
     <row r="13" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Update: Wrote miniparagraphs for nearly all analysis within matrix, which was also slightly tweaked
</commit_message>
<xml_diff>
--- a/templates/gap-analysis-template.xlsx
+++ b/templates/gap-analysis-template.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\ALL MY FILES\Documents\Personal Coding\Cybersecurity projects\controls-gap-analysis\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E549918-940C-4CC6-A618-98AB4544759A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934E1533-E874-4E9A-9DCD-8C0F1B234801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="8580" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$33</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -168,9 +171,6 @@
     <t>Data Management</t>
   </si>
   <si>
-    <t>On the "Digital services privacy notice" page of the council's website, the council lists out the personal information of residents they collect and process.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective A1 - </t>
     </r>
@@ -187,9 +187,6 @@
     </r>
   </si>
   <si>
-    <t>On the "Cookies and IP addresses" page of the council, they explain the Google Analytics cookies used are to collect information on how their sites are used, to compile reports and help improve the sites.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">NCSF Cyber Assessment Framework, Objective A3 - </t>
     </r>
@@ -319,9 +316,6 @@
     </r>
   </si>
   <si>
-    <t>H&amp;F's control room consists of around 1850 cameras throughout the borough, and have radio communications with the police. CCTV is used to ensure reducing crime rates. Residents can access CCTV footage according to their rights, and have to fill a form consisting of personal information and signing the application form.</t>
-  </si>
-  <si>
     <r>
       <t>ISO 27001 Annex A Control -</t>
     </r>
@@ -386,9 +380,6 @@
     <t>H&amp;F should implement a shorter timeout (25 or 30 minutes) to reduce the chance of an active activity being spotted by an unauthorised user. It also alerts the actual user to be aware that they should return as soon as possible if they have been inactive at some point.</t>
   </si>
   <si>
-    <t>H&amp;F must continue to maintain this practice, as its residents are aware of their personal information being processed, which is a requirement under the Data Protection Act 2018.</t>
-  </si>
-  <si>
     <t>H&amp;F must ensure that the records about their residents are up to date at all times, as required by the Data Protection Act 2018. Credit to them, they do attempt this by holding an annual canvass, contacting every property in the borough and checking for changes.</t>
   </si>
   <si>
@@ -404,18 +395,12 @@
     <t>The H&amp;F council mentions reasons for having non-stop CCTV, but that's a 24/7  intrusion which compromises privacy. If not done, H&amp;F must implement a backup system for their CCTV in the event of a shutdown.</t>
   </si>
   <si>
-    <t>H&amp;F must continue to comply with laws regularly to ensure they meet the necessary data security procedures. Breaching the law can have serious consequences such as fines &amp; distrust from the public.</t>
-  </si>
-  <si>
     <t>Surveilance</t>
   </si>
   <si>
     <t>Organisational Procedures</t>
   </si>
   <si>
-    <t xml:space="preserve"> H&amp;F council must continue to maintain regular testing of its systems to mitigate potential cybersecurity risks. However, any details about the security workers shouldn't be disclosed for security reasons (structure, personnel), as they manage personal and sensitive data.</t>
-  </si>
-  <si>
     <t>To log into your personal portal, you have to enter your correct email and password of your account.</t>
   </si>
   <si>
@@ -429,6 +414,24 @@
   </si>
   <si>
     <t>Low - Rateable values of property by law can be viewed by the public.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H&amp;F council must continue to maintain regular testing of its systems to mitigate potential cybersecurity risks. </t>
+  </si>
+  <si>
+    <t>On the "Digital services privacy notice" page of the council's website, the council lists out the personal information of residents they collect and process. It also lists  its reasoning for this later in the web page.</t>
+  </si>
+  <si>
+    <t>H&amp;F must continue to maintain this practice, as the reasoning for data being stored is part of the Data Protection Act 2018. Residents knowing what data is stored is part of GDPR.</t>
+  </si>
+  <si>
+    <t>The council’s "Cookies and IP addresses" page says Google Analytics cookies are used to track site usage, compile reports, and improve services. The data is anonymous and contains no personal information.</t>
+  </si>
+  <si>
+    <t>H&amp;F's control room consists of around 1850 cameras throughout the borough. CCTV is used to ensure reducing crime rates. Residents can access CCTV footage according to their rights, and have to fill a form consisting of personal information and signing the application form.</t>
+  </si>
+  <si>
+    <t>H&amp;F must continue to comply with laws regularly to ensure they meet the necessary data security procedures. Breaching the law can have serious consequences such as fines &amp; distrust from the public. Council must also maintain rigorous checks to system to mitigate the risk carried by the potential threat actor.</t>
   </si>
 </sst>
 </file>
@@ -514,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -526,9 +529,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -866,10 +866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C1E297-21ED-43A1-9A9E-ACD768065ED2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +907,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -917,16 +918,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -940,33 +941,33 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="198.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -977,13 +978,13 @@
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -991,19 +992,19 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,19 +1012,19 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1031,122 +1032,122 @@
         <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="153.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="166.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="165" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1154,7 +1155,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1162,7 +1163,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1170,7 +1171,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1178,7 +1179,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1186,7 +1187,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1194,7 +1195,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1202,7 +1203,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1210,7 +1211,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1218,7 +1219,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1226,7 +1227,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1234,7 +1235,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1242,7 +1243,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1250,7 +1251,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1258,7 +1259,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1266,7 +1267,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1274,7 +1275,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1282,7 +1283,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1290,7 +1291,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1298,7 +1299,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1307,6 +1308,13 @@
       <c r="F33" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A33" xr:uid="{86C1E297-21ED-43A1-9A9E-ACD768065ED2}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Data Management"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates: Made adjustments to the markdown files, and finished the Gap analysis report and the finalised the Matrix table
</commit_message>
<xml_diff>
--- a/templates/gap-analysis-template.xlsx
+++ b/templates/gap-analysis-template.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\ALL MY FILES\Documents\Personal Coding\Cybersecurity projects\controls-gap-analysis\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF95C82-D5C8-4E11-96F0-D6B43DAC8A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7B9C96-414B-484A-B5CC-34FEFA5F7ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="8580" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="317" xr2:uid="{BA46F687-07D1-4F5F-88F9-0B77A73535ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -341,9 +341,6 @@
     <t>Residual Risk</t>
   </si>
   <si>
-    <t>Medium - H&amp;F does mention reasons as to why they have the CCTV being watched 24/7. You access parts of it if you verify your details, which are compared to the records they have. However, privacy concerns arise due to non-stop activity monitoring, which can be perceived as intrusive.</t>
-  </si>
-  <si>
     <t>Pending council response</t>
   </si>
   <si>
@@ -428,17 +425,20 @@
     <t>The council’s "Cookies and IP addresses" page says Google Analytics cookies are used to track site usage, compile reports, and improve services. The data is anonymous and contains no personal information.</t>
   </si>
   <si>
-    <t>H&amp;F's control room consists of around 1850 cameras throughout the borough. CCTV is used to ensure reducing crime rates. Residents can access CCTV footage according to their rights, and have to fill a form consisting of personal information and signing the application form.</t>
-  </si>
-  <si>
     <t>H&amp;F must continue to comply with laws regularly to ensure they meet the necessary data security procedures. Breaching the law can have serious consequences such as fines &amp; distrust from the public. Council must also maintain rigorous checks to system to mitigate the risk carried by the potential threat actor.</t>
+  </si>
+  <si>
+    <t>H&amp;F's control room consists of around 1850 cameras throughout the borough. CCTV is used to ensure reducing crime rates.</t>
+  </si>
+  <si>
+    <t>Medium - H&amp;F does mention reasons as to why they have the CCTV being watched 24/7.  However, privacy concerns arise due to non-stop activity monitoring, which can be perceived as intrusive.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,13 +468,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -489,8 +482,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,8 +512,38 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC598CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -512,16 +551,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -529,6 +580,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -538,6 +628,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC598CE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -866,455 +961,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C1E297-21ED-43A1-9A9E-ACD768065ED2}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="54.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="13.7109375" style="8" customWidth="1"/>
+    <col min="2" max="3" width="50.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="50.7109375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="58.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    <row r="6" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="198.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="B10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
+    <row r="11" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="E11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="153.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="166.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="165" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="B12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="115.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="D12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A33" xr:uid="{86C1E297-21ED-43A1-9A9E-ACD768065ED2}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Data Management"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="D1:D33" xr:uid="{86C1E297-21ED-43A1-9A9E-ACD768065ED2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>